<commit_message>
add plants and new criteria
</commit_message>
<xml_diff>
--- a/data/scoring.xlsx
+++ b/data/scoring.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>group</t>
   </si>
@@ -28,6 +28,9 @@
     <t>splits</t>
   </si>
   <si>
+    <t>subspecies</t>
+  </si>
+  <si>
     <t>total</t>
   </si>
   <si>
@@ -35,6 +38,9 @@
   </si>
   <si>
     <t>realm</t>
+  </si>
+  <si>
+    <t>nbr_spp</t>
   </si>
   <si>
     <t>dragonflies</t>
@@ -123,7 +129,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -137,6 +143,9 @@
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -374,7 +383,7 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -383,10 +392,16 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
+      <c r="A2" s="1" t="s">
+        <v>10</v>
       </c>
       <c r="B2" s="3">
         <v>2.0</v>
@@ -400,47 +415,59 @@
       <c r="E2" s="3">
         <v>0.0</v>
       </c>
-      <c r="F2" s="1">
-        <f t="shared" ref="F2:F10" si="1">sum(B2:E2)</f>
+      <c r="F2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G2" s="1">
+        <f t="shared" ref="G2:G10" si="1">sum(B2:F2)</f>
+        <v>5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="1">
+        <v>6324.0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C3" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G3" s="1">
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="D3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F3" s="1">
-        <f t="shared" si="1"/>
-        <v>1</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="1" t="s">
-        <v>10</v>
+      <c r="J3" s="1">
+        <v>437644.0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>13</v>
+      <c r="A4" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="B4" s="3">
         <v>2.0</v>
@@ -451,77 +478,95 @@
       <c r="D4" s="3">
         <v>2.0</v>
       </c>
-      <c r="E4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="C5" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="1"/>
-        <v>3</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C6" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="E4" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G4" s="1">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="1">
+        <v>16517.0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1.0</v>
+      </c>
+      <c r="C5" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="H5" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="I5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J5" s="1">
+        <v>19207.0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G6" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
       <c r="H6" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="J6" s="1">
+        <v>8931.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>20</v>
+      <c r="A7" s="1" t="s">
+        <v>22</v>
       </c>
       <c r="B7" s="3">
         <v>2.0</v>
@@ -535,20 +580,26 @@
       <c r="E7" s="3">
         <v>0.0</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J7" s="1">
+        <v>6533.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="2" t="s">
-        <v>22</v>
+      <c r="A8" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B8" s="3">
         <v>2.0</v>
@@ -559,79 +610,98 @@
       <c r="D8" s="3">
         <v>2.0</v>
       </c>
-      <c r="E8" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="1">
+      <c r="E8" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J8" s="1">
+        <v>10585.0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F9" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G9" s="1">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E9" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="1">
+      <c r="I9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J9" s="1">
+        <v>8105.0</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E10" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G10" s="1">
         <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J10" s="1">
+        <v>11050.0</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
-      <c r="E11" s="5"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
update scores and make boxplots of scores
</commit_message>
<xml_diff>
--- a/data/scoring.xlsx
+++ b/data/scoring.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="31">
   <si>
     <t>group</t>
   </si>
@@ -25,12 +25,21 @@
     <t>authorship</t>
   </si>
   <si>
-    <t>splits</t>
+    <t>splits_time</t>
+  </si>
+  <si>
+    <t>splits_space</t>
   </si>
   <si>
     <t>subspecies</t>
   </si>
   <si>
+    <t>checklist</t>
+  </si>
+  <si>
+    <t>completeness</t>
+  </si>
+  <si>
     <t>total</t>
   </si>
   <si>
@@ -92,6 +101,9 @@
   </si>
   <si>
     <t>reptiles</t>
+  </si>
+  <si>
+    <t>fishes</t>
   </si>
 </sst>
 </file>
@@ -380,31 +392,40 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B2" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C2" s="3">
         <v>0.0</v>
@@ -416,28 +437,37 @@
         <v>0.0</v>
       </c>
       <c r="F2" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G2" s="1">
-        <f t="shared" ref="G2:G10" si="1">sum(B2:F2)</f>
-        <v>5</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>12</v>
+        <v>0.0</v>
+      </c>
+      <c r="G2" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H2" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>1.0</v>
       </c>
       <c r="J2" s="1">
+        <f t="shared" ref="J2:J11" si="1">SUM(B2:I2)</f>
+        <v>9</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M2" s="1">
         <v>6324.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B3" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C3" s="4">
         <v>1.0</v>
@@ -449,58 +479,76 @@
         <v>0.0</v>
       </c>
       <c r="F3" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G3" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="J3" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="1">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M3" s="1">
         <v>437644.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D4" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E4" s="5">
+        <v>0.0</v>
+      </c>
+      <c r="F4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G4" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H4" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I4" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="J4" s="1">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C4" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D4" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G4" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="M4" s="1">
         <v>16517.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B5" s="5">
         <v>1.0</v>
@@ -515,31 +563,40 @@
         <v>0.0</v>
       </c>
       <c r="F5" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G5" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G5" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H5" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="I5" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="J5" s="1">
         <f t="shared" si="1"/>
-        <v>4</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="1">
+        <v>9</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M5" s="1">
         <v>19207.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="C6" s="3">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="D6" s="3">
         <v>2.0</v>
@@ -548,160 +605,204 @@
         <v>0.0</v>
       </c>
       <c r="F6" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G6" s="1">
+        <v>0.0</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.0</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="1">
+        <v>8931.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.0</v>
+      </c>
+      <c r="G7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="H7" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M7" s="1">
+        <v>6533.0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F8" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="1">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M8" s="1">
+        <v>10585.0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="1">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J6" s="1">
-        <v>8931.0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D7" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E7" s="3">
-        <v>0.0</v>
-      </c>
-      <c r="F7" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="G7" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="1">
-        <v>6533.0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C8" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D8" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F8" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G8" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="1">
-        <v>10585.0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B9" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C9" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D9" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E9" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F9" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G9" s="1">
-        <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M9" s="1">
         <v>8105.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B10" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="1">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="K10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="C10" s="3">
-        <v>1.0</v>
-      </c>
-      <c r="D10" s="3">
-        <v>2.0</v>
-      </c>
-      <c r="E10" s="5">
-        <v>0.0</v>
-      </c>
-      <c r="F10" s="4">
-        <v>1.0</v>
-      </c>
-      <c r="G10" s="1">
+      <c r="L10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="M10" s="1">
+        <v>11050.0</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3.0</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2.0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="F11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G11" s="6"/>
+      <c r="H11" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="I11" s="6"/>
+      <c r="J11" s="1">
         <f t="shared" si="1"/>
-        <v>6</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="1">
-        <v>11050.0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
+        <v>8</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>

</xml_diff>